<commit_message>
Completed testing and fixed rounding errors
</commit_message>
<xml_diff>
--- a/Outputs/Treatment at T1 v. T2 (Unweighted)/Tables - Ordinal Variables - Treatment at T1 v. T2 (Unweighted) - Consume Social Media News (T2).xlsx
+++ b/Outputs/Treatment at T1 v. T2 (Unweighted)/Tables - Ordinal Variables - Treatment at T1 v. T2 (Unweighted) - Consume Social Media News (T2).xlsx
@@ -54157,107 +54157,107 @@
       </c>
       <c r="D481" t="inlineStr">
         <is>
-          <t>0.0%</t>
+          <t>nan%</t>
         </is>
       </c>
       <c r="E481" t="inlineStr">
         <is>
-          <t>0.0%</t>
+          <t>nan%</t>
         </is>
       </c>
       <c r="F481" t="inlineStr">
         <is>
-          <t>0.0%</t>
+          <t>nan%</t>
         </is>
       </c>
       <c r="G481" t="inlineStr">
         <is>
-          <t>0.0%</t>
+          <t>nan%</t>
         </is>
       </c>
       <c r="H481" t="inlineStr">
         <is>
-          <t>0.0%</t>
+          <t>nan%</t>
         </is>
       </c>
       <c r="I481" t="inlineStr">
         <is>
-          <t>0.0%</t>
+          <t>nan%</t>
         </is>
       </c>
       <c r="J481" t="inlineStr">
         <is>
-          <t>0.0%</t>
+          <t>nan%</t>
         </is>
       </c>
       <c r="K481" t="inlineStr">
         <is>
-          <t>0.0%</t>
+          <t>nan%</t>
         </is>
       </c>
       <c r="L481" t="inlineStr">
         <is>
-          <t>0.0%</t>
+          <t>nan%</t>
         </is>
       </c>
       <c r="M481" t="inlineStr">
         <is>
-          <t>0.0%</t>
+          <t>nan%</t>
         </is>
       </c>
       <c r="N481" t="inlineStr">
         <is>
-          <t>0.0%</t>
+          <t>nan%</t>
         </is>
       </c>
       <c r="O481" t="inlineStr">
         <is>
-          <t>0.0%</t>
+          <t>nan%</t>
         </is>
       </c>
       <c r="P481" t="inlineStr">
         <is>
-          <t>0.0%</t>
+          <t>nan%</t>
         </is>
       </c>
       <c r="Q481" t="inlineStr">
         <is>
-          <t>0.0%</t>
+          <t>nan%</t>
         </is>
       </c>
       <c r="R481" t="inlineStr">
         <is>
-          <t>0.0%</t>
+          <t>nan%</t>
         </is>
       </c>
       <c r="S481" t="inlineStr">
         <is>
-          <t>0.0%</t>
+          <t>nan%</t>
         </is>
       </c>
       <c r="T481" t="inlineStr">
         <is>
-          <t>0.0%</t>
+          <t>nan%</t>
         </is>
       </c>
       <c r="U481" t="inlineStr">
         <is>
-          <t>0.0%</t>
+          <t>nan%</t>
         </is>
       </c>
       <c r="V481" t="inlineStr">
         <is>
-          <t>0.0%</t>
+          <t>nan%</t>
         </is>
       </c>
       <c r="W481" t="inlineStr">
         <is>
-          <t>0.0%</t>
+          <t>nan%</t>
         </is>
       </c>
       <c r="X481" t="inlineStr">
         <is>
-          <t>0.0%</t>
+          <t>nan%</t>
         </is>
       </c>
     </row>
@@ -54271,107 +54271,107 @@
       </c>
       <c r="D482" t="inlineStr">
         <is>
-          <t>0.0%</t>
+          <t>nan%</t>
         </is>
       </c>
       <c r="E482" t="inlineStr">
         <is>
-          <t>0.0%</t>
+          <t>nan%</t>
         </is>
       </c>
       <c r="F482" t="inlineStr">
         <is>
-          <t>0.0%</t>
+          <t>nan%</t>
         </is>
       </c>
       <c r="G482" t="inlineStr">
         <is>
-          <t>0.0%</t>
+          <t>nan%</t>
         </is>
       </c>
       <c r="H482" t="inlineStr">
         <is>
-          <t>0.0%</t>
+          <t>nan%</t>
         </is>
       </c>
       <c r="I482" t="inlineStr">
         <is>
-          <t>0.0%</t>
+          <t>nan%</t>
         </is>
       </c>
       <c r="J482" t="inlineStr">
         <is>
-          <t>0.0%</t>
+          <t>nan%</t>
         </is>
       </c>
       <c r="K482" t="inlineStr">
         <is>
-          <t>0.0%</t>
+          <t>nan%</t>
         </is>
       </c>
       <c r="L482" t="inlineStr">
         <is>
-          <t>0.0%</t>
+          <t>nan%</t>
         </is>
       </c>
       <c r="M482" t="inlineStr">
         <is>
-          <t>0.0%</t>
+          <t>nan%</t>
         </is>
       </c>
       <c r="N482" t="inlineStr">
         <is>
-          <t>0.0%</t>
+          <t>nan%</t>
         </is>
       </c>
       <c r="O482" t="inlineStr">
         <is>
-          <t>0.0%</t>
+          <t>nan%</t>
         </is>
       </c>
       <c r="P482" t="inlineStr">
         <is>
-          <t>0.0%</t>
+          <t>nan%</t>
         </is>
       </c>
       <c r="Q482" t="inlineStr">
         <is>
-          <t>0.0%</t>
+          <t>nan%</t>
         </is>
       </c>
       <c r="R482" t="inlineStr">
         <is>
-          <t>0.0%</t>
+          <t>nan%</t>
         </is>
       </c>
       <c r="S482" t="inlineStr">
         <is>
-          <t>0.0%</t>
+          <t>nan%</t>
         </is>
       </c>
       <c r="T482" t="inlineStr">
         <is>
-          <t>0.0%</t>
+          <t>nan%</t>
         </is>
       </c>
       <c r="U482" t="inlineStr">
         <is>
-          <t>0.0%</t>
+          <t>nan%</t>
         </is>
       </c>
       <c r="V482" t="inlineStr">
         <is>
-          <t>0.0%</t>
+          <t>nan%</t>
         </is>
       </c>
       <c r="W482" t="inlineStr">
         <is>
-          <t>0.0%</t>
+          <t>nan%</t>
         </is>
       </c>
       <c r="X482" t="inlineStr">
         <is>
-          <t>0.0%</t>
+          <t>nan%</t>
         </is>
       </c>
     </row>

</xml_diff>